<commit_message>
Done....? Przechodzą wszystkie testy
</commit_message>
<xml_diff>
--- a/zpi-backend/src/test/resources/test_plik_pracownicy.xlsx
+++ b/zpi-backend/src/test/resources/test_plik_pracownicy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\zpi-student-project-management\zpi-backend\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EBCB30-3A73-45ED-9BBC-EE3299485B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6F681D-0183-438F-B95D-F644FA1FFB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0D141775-F52B-4CFE-9CEF-DBC76E6B4B4D}"/>
+    <workbookView xWindow="1680" yWindow="2235" windowWidth="21600" windowHeight="11295" xr2:uid="{0D141775-F52B-4CFE-9CEF-DBC76E6B4B4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -206,10 +206,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -527,7 +526,7 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,7 +704,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="1"/>
-      <c r="I6" s="2" t="s">
+      <c r="I6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -731,7 +730,7 @@
       <c r="G7" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -757,7 +756,7 @@
       <c r="G8" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="2" t="s">
+      <c r="I8" t="s">
         <v>36</v>
       </c>
     </row>
@@ -783,7 +782,7 @@
       <c r="G9" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" t="s">
         <v>37</v>
       </c>
     </row>
@@ -809,7 +808,7 @@
       <c r="G10" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" t="s">
         <v>38</v>
       </c>
     </row>
@@ -835,7 +834,7 @@
       <c r="G11" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -861,7 +860,7 @@
       <c r="G12" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" t="s">
         <v>40</v>
       </c>
     </row>
@@ -887,7 +886,7 @@
       <c r="G13" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" t="s">
         <v>35</v>
       </c>
     </row>
@@ -916,7 +915,7 @@
       <c r="H14" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="I14" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>